<commit_message>
redid demog testing with masked sfs and full dataset
</commit_message>
<xml_diff>
--- a/05.analyses/demography/dadi/2D/models/dadi_2D_results_summary.xlsx
+++ b/05.analyses/demography/dadi/2D/models/dadi_2D_results_summary.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/kasey_pham_ufl_edu/Documents/Grad School Documents/Projects/eucalyptus-hybrid-resequencing/05.analyses/demography/dadi/2D/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1181" documentId="11_F25DC773A252ABDACC1048CC295F61E45BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{048D7316-04DA-44C3-9621-54852FEF2F32}"/>
+  <xr:revisionPtr revIDLastSave="1508" documentId="11_F25DC773A252ABDACC1048CC295F61E45BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{773F6229-E593-4300-82E3-6D6D25320ED4}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-7275" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1308" yWindow="-108" windowWidth="21840" windowHeight="13176" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all model results" sheetId="1" r:id="rId1"/>
     <sheet name="calc templ" sheetId="8" r:id="rId2"/>
+    <sheet name="04 calc" sheetId="15" r:id="rId3"/>
+    <sheet name="01 calc" sheetId="16" r:id="rId4"/>
+    <sheet name="05 calc" sheetId="17" r:id="rId5"/>
+    <sheet name="06 calc" sheetId="19" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="75">
   <si>
     <t>Model</t>
   </si>
@@ -109,70 +113,6 @@
   </si>
   <si>
     <t>DERIVED PARAMETERS</t>
-  </si>
-  <si>
-    <r>
-      <t>nu</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1a</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>nu</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2a</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>nu</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1b</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>nu</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2b</t>
-    </r>
   </si>
   <si>
     <r>
@@ -437,9 +377,6 @@
     <t>MODEL:</t>
   </si>
   <si>
-    <t>TYPE:</t>
-  </si>
-  <si>
     <t>01.schange</t>
   </si>
   <si>
@@ -477,6 +414,126 @@
   </si>
   <si>
     <t>06.sec_contact_bottle_schange_thr_epoch</t>
+  </si>
+  <si>
+    <t>Run 1 Rep 12</t>
+  </si>
+  <si>
+    <t>Run 2 Rep 59</t>
+  </si>
+  <si>
+    <t>Run 3 Rep 73</t>
+  </si>
+  <si>
+    <t>Run 4 Rep 67</t>
+  </si>
+  <si>
+    <t>Run 3 Rep 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run 4 </t>
+  </si>
+  <si>
+    <r>
+      <t>nu</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>nu</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>nu</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1m</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>nu</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2m</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>nu</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1f</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>nu</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2f</t>
+    </r>
+  </si>
+  <si>
+    <t>MIGR PERIOD</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -524,7 +581,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -549,8 +606,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="34">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -931,11 +1024,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -962,7 +1099,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -990,6 +1126,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1005,9 +1149,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1017,16 +1158,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1037,6 +1172,33 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1324,15 +1486,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" customWidth="1"/>
     <col min="15" max="17" width="7" bestFit="1" customWidth="1"/>
@@ -1347,37 +1510,37 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="44" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="42" t="s">
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="48"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="55"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
@@ -1412,26 +1575,26 @@
         <v>5</v>
       </c>
       <c r="L2" s="8"/>
-      <c r="M2" s="43" t="s">
+      <c r="M2" s="42" t="s">
         <v>14</v>
       </c>
       <c r="N2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="T2" s="7" t="s">
         <v>9</v>
@@ -1439,88 +1602,418 @@
       <c r="U2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="V2" s="43" t="s">
+      <c r="V2" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="43" t="s">
+      <c r="W2" s="42" t="s">
         <v>12</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="B3" s="48">
+        <v>-100346.1</v>
+      </c>
+      <c r="C3">
+        <v>-119954.2</v>
+      </c>
+      <c r="D3">
+        <v>-119405.3</v>
+      </c>
+      <c r="E3">
+        <v>-102060.1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>-108924.9</v>
+      </c>
+      <c r="G3" s="43">
+        <v>200702.2</v>
+      </c>
+      <c r="H3">
+        <v>239918.4</v>
+      </c>
+      <c r="I3">
+        <v>238820.6</v>
+      </c>
+      <c r="J3">
+        <v>204130.2</v>
+      </c>
+      <c r="K3" s="4">
+        <v>217859.7</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3">
+        <v>336964</v>
+      </c>
+      <c r="N3">
+        <v>0.1497</v>
+      </c>
+      <c r="O3">
+        <v>3.7086999999999999</v>
+      </c>
+      <c r="R3">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="S3">
+        <v>1.01E-2</v>
+      </c>
+      <c r="V3">
+        <v>2.3199999999999998E-2</v>
+      </c>
       <c r="X3" s="4"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>-149144.5</v>
+      </c>
+      <c r="C4" s="50">
+        <v>-118835.8</v>
+      </c>
+      <c r="D4">
+        <v>-120897.2</v>
+      </c>
+      <c r="E4">
+        <v>-175540.5</v>
+      </c>
+      <c r="F4" s="4">
+        <v>-189346.5</v>
+      </c>
+      <c r="G4">
+        <v>298304.90000000002</v>
+      </c>
+      <c r="H4" s="43">
+        <v>237687.7</v>
+      </c>
+      <c r="I4">
+        <v>241810.4</v>
+      </c>
+      <c r="J4">
+        <v>351097</v>
+      </c>
+      <c r="K4" s="4">
+        <v>378708.9</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M4">
+        <v>315612.09999999998</v>
+      </c>
+      <c r="N4">
+        <v>0.50529999999999997</v>
+      </c>
+      <c r="O4">
+        <v>0.3014</v>
+      </c>
+      <c r="P4">
+        <v>8.3599999999999994E-2</v>
+      </c>
+      <c r="Q4">
+        <v>1.0822000000000001</v>
+      </c>
+      <c r="R4">
+        <v>0.17249999999999999</v>
+      </c>
+      <c r="S4">
+        <v>2.7E-2</v>
+      </c>
+      <c r="V4">
+        <v>2.6700000000000002E-2</v>
+      </c>
+      <c r="W4">
+        <v>3.2099999999999997E-2</v>
+      </c>
       <c r="X4" s="4"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="X5" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <v>-248327.6</v>
+      </c>
+      <c r="C5">
+        <v>-1213186</v>
+      </c>
+      <c r="D5">
+        <v>-411871.9</v>
+      </c>
+      <c r="E5" s="49">
+        <v>-228936.9</v>
+      </c>
+      <c r="F5" s="4">
+        <v>-1124581</v>
+      </c>
+      <c r="G5">
+        <v>496673.2</v>
+      </c>
+      <c r="H5">
+        <v>2426391</v>
+      </c>
+      <c r="I5">
+        <v>823761.9</v>
+      </c>
+      <c r="J5" s="43">
+        <v>457891.8</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2249180</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M5">
+        <v>219902.3</v>
+      </c>
+      <c r="N5">
+        <v>0.72989999999999999</v>
+      </c>
+      <c r="O5">
+        <v>21.985199999999999</v>
+      </c>
+      <c r="P5">
+        <v>2.8016000000000001</v>
+      </c>
+      <c r="Q5">
+        <v>0.32029999999999997</v>
+      </c>
+      <c r="R5">
+        <v>0.1149</v>
+      </c>
+      <c r="S5">
+        <v>0.96279999999999999</v>
+      </c>
+      <c r="V5">
+        <v>8.2699999999999996E-2</v>
+      </c>
+      <c r="W5">
+        <v>7.6300000000000007E-2</v>
+      </c>
+      <c r="X5" s="4">
+        <v>6.0400000000000002E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="B6">
+        <v>-93094.8</v>
+      </c>
+      <c r="C6">
+        <v>-86262.81</v>
+      </c>
+      <c r="D6" s="45">
+        <v>-81001.600000000006</v>
+      </c>
+      <c r="E6">
+        <v>-104189.1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>-131517.29999999999</v>
+      </c>
+      <c r="G6">
+        <v>186205.6</v>
+      </c>
+      <c r="H6">
+        <v>172541.6</v>
+      </c>
+      <c r="I6" s="43">
+        <v>162019.20000000001</v>
+      </c>
+      <c r="J6">
+        <v>208394.1</v>
+      </c>
+      <c r="K6" s="4">
+        <v>263050.59999999998</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M6">
+        <v>71968.69</v>
+      </c>
+      <c r="N6">
+        <v>3.1768000000000001</v>
+      </c>
+      <c r="O6">
+        <v>9.5620999999999992</v>
+      </c>
+      <c r="R6">
+        <v>0.1053</v>
+      </c>
+      <c r="S6">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="T6">
+        <v>3.0836000000000001</v>
+      </c>
+      <c r="U6">
+        <v>5.4648000000000003</v>
+      </c>
+      <c r="V6">
+        <v>5.3705999999999996</v>
+      </c>
+      <c r="W6">
+        <v>0.14280000000000001</v>
+      </c>
       <c r="X6" s="4"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7">
+        <v>-151874.79999999999</v>
+      </c>
+      <c r="C7">
+        <v>-117330.3</v>
+      </c>
+      <c r="D7">
+        <v>-98864.34</v>
+      </c>
+      <c r="E7" s="46">
+        <v>-86270.55</v>
+      </c>
+      <c r="F7" s="4">
+        <v>-167668</v>
+      </c>
+      <c r="G7">
+        <v>303769.5</v>
+      </c>
+      <c r="H7">
+        <v>234680.6</v>
+      </c>
+      <c r="I7">
+        <v>197748.7</v>
+      </c>
+      <c r="J7" s="43">
+        <v>172561.1</v>
+      </c>
+      <c r="K7" s="4">
+        <v>335356.09999999998</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
+      <c r="M7">
+        <v>177855.6</v>
+      </c>
+      <c r="N7">
+        <v>0.78890000000000005</v>
+      </c>
+      <c r="O7">
+        <v>4.1205999999999996</v>
+      </c>
+      <c r="P7">
+        <v>1.1295999999999999</v>
+      </c>
+      <c r="Q7">
+        <v>6.1315</v>
+      </c>
+      <c r="R7">
+        <v>5.6300000000000003E-2</v>
+      </c>
+      <c r="S7">
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="T7">
+        <v>8.5219000000000005</v>
+      </c>
+      <c r="U7">
+        <v>5.9484000000000004</v>
+      </c>
+      <c r="V7">
+        <v>1.3299000000000001</v>
+      </c>
+      <c r="W7">
+        <v>7.4399999999999994E-2</v>
+      </c>
       <c r="X7" s="4"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="5">
+        <v>-97721.84</v>
+      </c>
+      <c r="C8" s="5">
+        <v>-96668.25</v>
+      </c>
+      <c r="D8" s="47">
+        <v>-91732.12</v>
+      </c>
+      <c r="E8" s="5">
+        <v>-114255.8</v>
+      </c>
+      <c r="F8" s="6">
+        <v>-132210</v>
+      </c>
+      <c r="G8" s="5">
+        <v>195465.7</v>
+      </c>
+      <c r="H8" s="5">
+        <v>193358.5</v>
+      </c>
+      <c r="I8" s="44">
+        <v>183486.2</v>
+      </c>
+      <c r="J8" s="5">
+        <v>228533.6</v>
+      </c>
+      <c r="K8" s="6">
+        <v>264441.90000000002</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="6"/>
+      <c r="M8" s="5">
+        <v>20816.03</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="O8" s="5">
+        <v>1.5760000000000001</v>
+      </c>
+      <c r="P8" s="5">
+        <v>8.2385999999999999</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>13.714399999999999</v>
+      </c>
+      <c r="R8" s="5">
+        <v>0.1104</v>
+      </c>
+      <c r="S8" s="5">
+        <v>5.45E-2</v>
+      </c>
+      <c r="T8" s="5">
+        <v>1.3498000000000001</v>
+      </c>
+      <c r="U8" s="5">
+        <v>0.91690000000000005</v>
+      </c>
+      <c r="V8" s="5">
+        <v>1.35E-2</v>
+      </c>
+      <c r="W8" s="5">
+        <v>25.9312</v>
+      </c>
+      <c r="X8" s="6">
+        <v>0.11700000000000001</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1535,10 +2028,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB1F3D2-B500-4738-93FB-A5F3BE4B45CC}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1561,34 +2054,34 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+        <v>47</v>
+      </c>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
       <c r="F1" s="9" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="59"/>
-      <c r="F3" s="50" t="s">
+      <c r="B3" s="57"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="63"/>
+      <c r="F3" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52"/>
-      <c r="J3" s="50" t="s">
+      <c r="G3" s="57"/>
+      <c r="H3" s="58"/>
+      <c r="J3" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="52"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="58"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
@@ -1596,7 +2089,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>21</v>
@@ -1605,7 +2098,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>21</v>
@@ -1615,254 +2108,288 @@
         <v>15</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M4" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="48" x14ac:dyDescent="0.35">
-      <c r="A5" s="36" t="s">
+    <row r="5" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="35" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D5" s="20"/>
-      <c r="F5" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="35" t="s">
-        <v>35</v>
+      <c r="F5" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>31</v>
       </c>
       <c r="H5" s="20">
         <v>4.9300000000000001E-9</v>
       </c>
-      <c r="J5" s="53" t="s">
+      <c r="J5" s="65" t="s">
         <v>16</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="L5" s="23"/>
-      <c r="M5" s="37">
+      <c r="M5" s="36">
         <f>D5/(4*H5*H6*H9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="51.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="13"/>
-      <c r="F6" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="35" t="s">
-        <v>42</v>
+      <c r="B6" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="69"/>
+      <c r="D6" s="72"/>
+      <c r="F6" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>38</v>
       </c>
       <c r="H6" s="20">
         <v>10</v>
       </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="25"/>
-      <c r="M6" s="38">
+      <c r="J6" s="66"/>
+      <c r="K6" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" s="28"/>
+      <c r="M6" s="78">
         <f>D6*M5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A7" s="54"/>
-      <c r="B7" t="s">
-        <v>25</v>
+      <c r="A7" s="66"/>
+      <c r="B7" s="70" t="s">
+        <v>68</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="13"/>
       <c r="F7" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H7" s="13">
         <v>603301446</v>
       </c>
-      <c r="J7" s="54"/>
-      <c r="K7" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="25"/>
-      <c r="M7" s="38">
+      <c r="J7" s="66"/>
+      <c r="K7" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" s="24"/>
+      <c r="M7" s="79">
         <f>D7*M5</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A8" s="54"/>
-      <c r="B8" t="s">
-        <v>26</v>
+      <c r="A8" s="66"/>
+      <c r="B8" s="70" t="s">
+        <v>69</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="13"/>
       <c r="F8" s="16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="13">
         <f>(8732510/600502230)*(1066040/1226278)</f>
         <v>1.2641803364126243E-2</v>
       </c>
-      <c r="J8" s="54"/>
-      <c r="K8" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="L8" s="25"/>
-      <c r="M8" s="38">
+      <c r="J8" s="66"/>
+      <c r="K8" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="24"/>
+      <c r="M8" s="79">
         <f>D8*M5</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="55"/>
-      <c r="B9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="20"/>
-      <c r="F9" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="32">
+      <c r="A9" s="66"/>
+      <c r="B9" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="13"/>
+      <c r="F9" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="31">
         <f>H7*H8</f>
         <v>7626818.2496250272</v>
       </c>
-      <c r="J9" s="55"/>
-      <c r="K9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" s="27"/>
-      <c r="M9" s="39">
+      <c r="J9" s="66"/>
+      <c r="K9" s="76" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="24"/>
+      <c r="M9" s="79">
         <f>D9*M5</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="66"/>
+      <c r="B10" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="13"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="76" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" s="24"/>
+      <c r="M10" s="79">
+        <f>D10*M5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="73"/>
+      <c r="B11" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="20"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="26"/>
+      <c r="M11" s="79">
+        <f>D11*M5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="J10" s="53" t="s">
+      <c r="B12" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="J12" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="K12" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="39" t="e">
+        <f>IF(G1="M",(D12*M8)/(2*M5),(D12*M10)/(2*M5))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="60"/>
+      <c r="B13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="38" t="e">
+        <f>IF(G1="M",(D13*M9)/(M5*2),(D13*M11)/(M5*2))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="28.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="13"/>
+      <c r="J14" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="37">
+        <f>2*D14*M5*H6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" s="66"/>
+      <c r="B15" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="13"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" s="37">
+        <f>2*D15*M5*H6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="67"/>
+      <c r="B16" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="M10" s="40" t="e">
-        <f>IF(G1="SIZE",M9/(2*D10),M7/(2*D10))</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="55"/>
-      <c r="B11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="M11" s="39" t="e">
-        <f>IF(G1="SIZE",D11/(M8*2),D11/(M6*2))</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="53" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="13"/>
-      <c r="J12" s="53" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="L12" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="M12" s="38">
-        <f>2*D12*M5*H6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A13" s="54"/>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="13"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="L13" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="M13" s="38">
-        <f>2*D13*M5*H6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="56"/>
-      <c r="B14" s="19" t="s">
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="L14" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="M14" s="41">
-        <f>2*D14*M5*H6</f>
+      <c r="M16" s="40">
+        <f>2*D16*M5*H6</f>
         <v>0</v>
       </c>
     </row>
@@ -1870,14 +2397,1637 @@
   <mergeCells count="10">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="J3:M3"/>
-    <mergeCell ref="J5:J9"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="J12:J14"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="J5:J11"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="J14:J16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{040C5F90-B158-4862-AA5B-6C31B78B8164}">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="4.77734375" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="F1" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="57"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="63"/>
+      <c r="F3" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58"/>
+      <c r="J3" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="58"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="21"/>
+      <c r="K4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="20">
+        <v>71968.69</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="20">
+        <v>4.9300000000000001E-9</v>
+      </c>
+      <c r="J5" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="23"/>
+      <c r="M5" s="36">
+        <f>D5/(4*H5*H6*H9)</f>
+        <v>47851.250298851177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="51.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="69"/>
+      <c r="D6" s="72">
+        <v>3.1768000000000001</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="20">
+        <v>10</v>
+      </c>
+      <c r="J6" s="66"/>
+      <c r="K6" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" s="28"/>
+      <c r="M6" s="78">
+        <f>D6*M5</f>
+        <v>152013.85194939043</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A7" s="66"/>
+      <c r="B7" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="13">
+        <v>9.5620999999999992</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="13">
+        <v>603301446</v>
+      </c>
+      <c r="J7" s="66"/>
+      <c r="K7" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" s="24"/>
+      <c r="M7" s="79">
+        <f>D7*M5</f>
+        <v>457558.44048264477</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A8" s="66"/>
+      <c r="B8" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="13"/>
+      <c r="F8" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="13">
+        <f>(8732510/600502230)*(1066040/1226278)</f>
+        <v>1.2641803364126243E-2</v>
+      </c>
+      <c r="J8" s="66"/>
+      <c r="K8" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="24"/>
+      <c r="M8" s="79">
+        <f>D8*M5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="66"/>
+      <c r="B9" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="13"/>
+      <c r="F9" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="31">
+        <f>H7*H8</f>
+        <v>7626818.2496250272</v>
+      </c>
+      <c r="J9" s="66"/>
+      <c r="K9" s="76" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="24"/>
+      <c r="M9" s="79">
+        <f>D9*M5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="66"/>
+      <c r="B10" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="13">
+        <v>0.1053</v>
+      </c>
+      <c r="J10" s="66"/>
+      <c r="K10" s="76" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" s="24"/>
+      <c r="M10" s="79">
+        <f>D10*M5</f>
+        <v>5038.7366564690292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="73"/>
+      <c r="B11" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="20">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="J11" s="73"/>
+      <c r="K11" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="26"/>
+      <c r="M11" s="79">
+        <f>D11*M5</f>
+        <v>1894.9095118345067</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="13">
+        <v>3.0836000000000001</v>
+      </c>
+      <c r="J12" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="39">
+        <f>IF(G1="M",(D12*M8)/(2*M5),(D12*M10)/(2*M5))</f>
+        <v>0.16235154000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="60"/>
+      <c r="B13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="20">
+        <v>5.4648000000000003</v>
+      </c>
+      <c r="J13" s="73"/>
+      <c r="K13" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="38">
+        <f>IF(G1="M",(D13*M9)/(M5*2),(D13*M11)/(M5*2))</f>
+        <v>0.10820304000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="28.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="13">
+        <v>5.3705999999999996</v>
+      </c>
+      <c r="J14" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="37">
+        <f>2*D14*M5*H6</f>
+        <v>5139798.4971002024</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" s="66"/>
+      <c r="B15" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="13">
+        <v>0.14280000000000001</v>
+      </c>
+      <c r="J15" s="66"/>
+      <c r="K15" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" s="37">
+        <f>2*D15*M5*H6</f>
+        <v>136663.17085351897</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="67"/>
+      <c r="B16" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" s="40">
+        <f>2*D16*M5*H6</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="J5:J11"/>
+    <mergeCell ref="A6:A11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7910FDE-95EA-4B4D-B1A0-05B30AE6AB51}">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="4.77734375" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="F1" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="57"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="63"/>
+      <c r="F3" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58"/>
+      <c r="J3" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="58"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="21"/>
+      <c r="K4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="20">
+        <v>336964</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="20">
+        <v>4.9300000000000001E-9</v>
+      </c>
+      <c r="J5" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="23"/>
+      <c r="M5" s="36">
+        <f>D5/(4*H5*H6*H9)</f>
+        <v>224043.93779714606</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="51.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="69"/>
+      <c r="D6" s="72">
+        <v>0.1497</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="20">
+        <v>10</v>
+      </c>
+      <c r="J6" s="66"/>
+      <c r="K6" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" s="28"/>
+      <c r="M6" s="78">
+        <f>D6*M5</f>
+        <v>33539.377488232763</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A7" s="66"/>
+      <c r="B7" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="13">
+        <v>3.7086999999999999</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="13">
+        <v>603301446</v>
+      </c>
+      <c r="J7" s="66"/>
+      <c r="K7" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" s="24"/>
+      <c r="M7" s="79">
+        <f>D7*M5</f>
+        <v>830911.75210827554</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A8" s="66"/>
+      <c r="B8" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="13"/>
+      <c r="F8" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="13">
+        <f>(8732510/600502230)*(1066040/1226278)</f>
+        <v>1.2641803364126243E-2</v>
+      </c>
+      <c r="J8" s="66"/>
+      <c r="K8" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="24"/>
+      <c r="M8" s="79">
+        <f>D8*M5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="66"/>
+      <c r="B9" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="13"/>
+      <c r="F9" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="31">
+        <f>H7*H8</f>
+        <v>7626818.2496250272</v>
+      </c>
+      <c r="J9" s="66"/>
+      <c r="K9" s="76" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="24"/>
+      <c r="M9" s="79">
+        <f>D9*M5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="66"/>
+      <c r="B10" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="13">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="J10" s="66"/>
+      <c r="K10" s="76" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" s="24"/>
+      <c r="M10" s="79">
+        <f>D10*M5</f>
+        <v>11157.388102297873</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="73"/>
+      <c r="B11" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="20">
+        <v>1.01E-2</v>
+      </c>
+      <c r="J11" s="73"/>
+      <c r="K11" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="26"/>
+      <c r="M11" s="79">
+        <f>D11*M5</f>
+        <v>2262.8437717511752</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="J12" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="39">
+        <f>IF(G1="M",(D12*M8)/(2*M5),(D12*M10)/(2*M5))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="60"/>
+      <c r="B13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="38">
+        <f>IF(G1="M",(D13*M9)/(M5*2),(D13*M11)/(M5*2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="28.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="13">
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="J14" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="37">
+        <f>2*D14*M5*H6</f>
+        <v>103956.38713787578</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" s="66"/>
+      <c r="B15" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="13"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" s="37">
+        <f>2*D15*M5*H6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="67"/>
+      <c r="B16" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" s="40">
+        <f>2*D16*M5*H6</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="J5:J11"/>
+    <mergeCell ref="A6:A11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CAB648-A05B-4C48-814E-9BD2F732E49B}">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="4.77734375" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="80" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="F1" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="57"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="63"/>
+      <c r="F3" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58"/>
+      <c r="J3" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="58"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="21"/>
+      <c r="K4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="20">
+        <v>177855.6</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="20">
+        <v>4.9300000000000001E-9</v>
+      </c>
+      <c r="J5" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="23"/>
+      <c r="M5" s="36">
+        <f>D5/(4*H5*H6*H9)</f>
+        <v>118254.38024024552</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="51.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="69"/>
+      <c r="D6" s="72">
+        <v>0.78890000000000005</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="20">
+        <v>10</v>
+      </c>
+      <c r="J6" s="66"/>
+      <c r="K6" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" s="28"/>
+      <c r="M6" s="78">
+        <f>D6*M5</f>
+        <v>93290.880571529691</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A7" s="66"/>
+      <c r="B7" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="13">
+        <v>4.1205999999999996</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="13">
+        <v>603301446</v>
+      </c>
+      <c r="J7" s="66"/>
+      <c r="K7" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" s="24"/>
+      <c r="M7" s="79">
+        <f>D7*M5</f>
+        <v>487278.99921795563</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A8" s="66"/>
+      <c r="B8" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="13">
+        <v>1.1295999999999999</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="13">
+        <f>(8732510/600502230)*(1066040/1226278)</f>
+        <v>1.2641803364126243E-2</v>
+      </c>
+      <c r="J8" s="66"/>
+      <c r="K8" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="24"/>
+      <c r="M8" s="79">
+        <f>D8*M5</f>
+        <v>133580.14791938133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="66"/>
+      <c r="B9" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="13">
+        <v>6.1315</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="31">
+        <f>H7*H8</f>
+        <v>7626818.2496250272</v>
+      </c>
+      <c r="J9" s="66"/>
+      <c r="K9" s="76" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="24"/>
+      <c r="M9" s="79">
+        <f>D9*M5</f>
+        <v>725076.73244306538</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="66"/>
+      <c r="B10" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="13">
+        <v>5.6300000000000003E-2</v>
+      </c>
+      <c r="J10" s="66"/>
+      <c r="K10" s="76" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" s="24"/>
+      <c r="M10" s="79">
+        <f>D10*M5</f>
+        <v>6657.7216075258229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="73"/>
+      <c r="B11" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="20">
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="J11" s="73"/>
+      <c r="K11" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="26"/>
+      <c r="M11" s="79">
+        <f>D11*M5</f>
+        <v>2897.2323158860154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="13">
+        <v>8.5219000000000005</v>
+      </c>
+      <c r="J12" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="39">
+        <f>IF(G1="M",(D12*M8)/(2*M5),(D12*M10)/(2*M5))</f>
+        <v>0.23989148500000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="60"/>
+      <c r="B13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="20">
+        <v>5.9484000000000004</v>
+      </c>
+      <c r="J13" s="73"/>
+      <c r="K13" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="38">
+        <f>IF(G1="M",(D13*M9)/(M5*2),(D13*M11)/(M5*2))</f>
+        <v>7.2867899999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="28.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="13">
+        <v>1.3299000000000001</v>
+      </c>
+      <c r="J14" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="37">
+        <f>2*D14*M5*H6</f>
+        <v>3145330.0056300503</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" s="66"/>
+      <c r="B15" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="13">
+        <v>7.4399999999999994E-2</v>
+      </c>
+      <c r="J15" s="66"/>
+      <c r="K15" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" s="37">
+        <f>2*D15*M5*H6</f>
+        <v>175962.51779748531</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="67"/>
+      <c r="B16" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" s="40">
+        <f>2*D16*M5*H6</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="J5:J11"/>
+    <mergeCell ref="A6:A11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C638186B-6157-4ADF-97F4-54F4EBDD73BB}">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="4.77734375" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="80" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="F1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="57"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="63"/>
+      <c r="F3" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58"/>
+      <c r="J3" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="58"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="21"/>
+      <c r="K4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="20">
+        <v>20816.03</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="20">
+        <v>4.9300000000000001E-9</v>
+      </c>
+      <c r="J5" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="23"/>
+      <c r="M5" s="36">
+        <f>D5/(4*H5*H6*H9)</f>
+        <v>13840.366717226547</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="51.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="69"/>
+      <c r="D6" s="72">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="20">
+        <v>10</v>
+      </c>
+      <c r="J6" s="66"/>
+      <c r="K6" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" s="28"/>
+      <c r="M6" s="78">
+        <f>D6*M5</f>
+        <v>10214.190637313191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A7" s="66"/>
+      <c r="B7" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="13">
+        <v>1.5760000000000001</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="13">
+        <v>603301446</v>
+      </c>
+      <c r="J7" s="66"/>
+      <c r="K7" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" s="24"/>
+      <c r="M7" s="79">
+        <f>D7*M5</f>
+        <v>21812.41794634904</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A8" s="66"/>
+      <c r="B8" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="13">
+        <v>8.2385999999999999</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="13">
+        <f>(8732510/600502230)*(1066040/1226278)</f>
+        <v>1.2641803364126243E-2</v>
+      </c>
+      <c r="J8" s="66"/>
+      <c r="K8" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="24"/>
+      <c r="M8" s="79">
+        <f>D8*M5</f>
+        <v>114025.24523654263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="66"/>
+      <c r="B9" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="13">
+        <v>13.714399999999999</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="31">
+        <f>H7*H8</f>
+        <v>7626818.2496250272</v>
+      </c>
+      <c r="J9" s="66"/>
+      <c r="K9" s="76" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="24"/>
+      <c r="M9" s="79">
+        <f>D9*M5</f>
+        <v>189812.32530673174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="66"/>
+      <c r="B10" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="13">
+        <v>0.1104</v>
+      </c>
+      <c r="J10" s="66"/>
+      <c r="K10" s="76" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" s="24"/>
+      <c r="M10" s="79">
+        <f>D10*M5</f>
+        <v>1527.9764855818107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="73"/>
+      <c r="B11" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="20">
+        <v>5.45E-2</v>
+      </c>
+      <c r="J11" s="73"/>
+      <c r="K11" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="26"/>
+      <c r="M11" s="79">
+        <f>D11*M5</f>
+        <v>754.29998608884682</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="13">
+        <v>1.3498000000000001</v>
+      </c>
+      <c r="J12" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="39">
+        <f>IF(G1="M",(D12*M8)/(2*M5),(D12*M10)/(2*M5))</f>
+        <v>5.5602311400000008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="60"/>
+      <c r="B13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="20">
+        <v>0.91690000000000005</v>
+      </c>
+      <c r="J13" s="73"/>
+      <c r="K13" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="38">
+        <f>IF(G1="M",(D13*M9)/(M5*2),(D13*M11)/(M5*2))</f>
+        <v>6.2873666800000008</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="28.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="13">
+        <v>1.35E-2</v>
+      </c>
+      <c r="J14" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="37">
+        <f>2*D14*M5*H6</f>
+        <v>3736.8990136511679</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" s="66"/>
+      <c r="B15" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="13">
+        <v>25.9312</v>
+      </c>
+      <c r="J15" s="66"/>
+      <c r="K15" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" s="37">
+        <f>2*D15*M5*H6</f>
+        <v>7177946.3483549003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="67"/>
+      <c r="B16" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="J16" s="67"/>
+      <c r="K16" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" s="40">
+        <f>2*D16*M5*H6</f>
+        <v>32386.458118310118</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="J5:J11"/>
+    <mergeCell ref="A6:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>